<commit_message>
[Md Ahsanullah] Add: added financial statement scripts for all companies
</commit_message>
<xml_diff>
--- a/Excel output files/Financial Statement Output.xlsx
+++ b/Excel output files/Financial Statement Output.xlsx
@@ -23,28 +23,28 @@
     <x:t>Value</x:t>
   </x:si>
   <x:si>
-    <x:t>Total Net Worth (Total Equity)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Positive</x:t>
-  </x:si>
-  <x:si>
     <x:t>Profitable in latest Financial Statement (Latest Full Year)</x:t>
   </x:si>
   <x:si>
     <x:t>Yes</x:t>
   </x:si>
   <x:si>
+    <x:t>Total Net Worth (Total Equity)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Negative</x:t>
+  </x:si>
+  <x:si>
     <x:t>Current Ratio</x:t>
   </x:si>
   <x:si>
-    <x:t>1.50</x:t>
+    <x:t>0.34</x:t>
   </x:si>
   <x:si>
     <x:t>Gearing Ratio</x:t>
   </x:si>
   <x:si>
-    <x:t>2.00</x:t>
+    <x:t>-1.53</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1027,7 +1027,7 @@
       <x:selection activeCell="A5" sqref="A5 A5:A5"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="37.425" defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultColWidth="50.21625" defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="23" style="1" customWidth="1"/>
     <x:col min="2" max="2" width="15.428571" style="1" customWidth="1"/>

</xml_diff>